<commit_message>
Entrega Final – laboratorio 4
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4.xlsx
+++ b/Docs/Tablas Lab 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Datos y Algoritmos\-LabSorts-S02-G03\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E197636-5D23-49AC-AB0F-C814FF421F77}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C038B693-803A-40D7-AC7B-05AF2DF5CA94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <r>
       <t>T</t>
@@ -79,12 +79,27 @@
       <t>amaño de la muestra (ARRAYLIST)</t>
     </r>
   </si>
+  <si>
+    <t>468.75</t>
+  </si>
+  <si>
+    <t>2062.5</t>
+  </si>
+  <si>
+    <t>10875.0</t>
+  </si>
+  <si>
+    <t>34718.75</t>
+  </si>
+  <si>
+    <t>150375.0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +164,31 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -362,31 +402,6 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -459,7 +474,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -526,7 +541,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -613,7 +628,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -664,34 +679,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>484.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>1843.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>8093.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>32015.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>138140.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>575031.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>720000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>1295031.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>2015031.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>2735031.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,7 +796,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -832,34 +847,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>625015625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>720000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>625735625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>626455625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>1252191250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -948,7 +963,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -999,34 +1014,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>46.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>312.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>734.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>1781.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>4125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>12765.625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
+                  <c:v>26265.625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>53432.324000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1126,7 +1141,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1164,7 +1179,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1248,7 +1263,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1286,7 +1301,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1328,7 +1343,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1365,7 +1380,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1374,7 +1389,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1441,7 +1456,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1528,7 +1543,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1579,34 +1594,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>39625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>316906.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>720000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>1036906.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90</c:v>
+                  <c:v>1756906.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>2793812.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>110</c:v>
+                  <c:v>4550718.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120</c:v>
+                  <c:v>7344531.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130</c:v>
+                  <c:v>11895250</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>19239781.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1696,7 +1711,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1708,34 +1723,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>37031.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>294046.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>331078.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>625125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>956203.125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>1581328.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>2537531.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68</c:v>
+                  <c:v>4118859.375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>6656390.625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>10775250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1747,34 +1762,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>37031.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>294046.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>331078.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>625125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>956203.125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>1581328.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>2537531.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68</c:v>
+                  <c:v>4118859.375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>6656390.625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>10775250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1863,7 +1878,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1914,34 +1929,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>1890.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>10375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>44968.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>204546.875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>204556.875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>118</c:v>
+                  <c:v>204566.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>128</c:v>
+                  <c:v>204576.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>138</c:v>
+                  <c:v>204586.875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>148</c:v>
+                  <c:v>204596.875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>204606.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2041,7 +2056,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2079,7 +2094,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -2163,7 +2178,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2201,7 +2216,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -2243,7 +2258,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2280,7 +2295,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2289,7 +2304,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2356,7 +2371,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2444,7 +2459,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2495,34 +2510,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>484.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>1843.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>8093.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>32015.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>138140.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>575031.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>720000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>1295031.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>2015031.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>2735031.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2612,7 +2627,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2663,34 +2678,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>39625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>316906.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>720000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>1036906.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90</c:v>
+                  <c:v>1756906.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>2793812.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>110</c:v>
+                  <c:v>4550718.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120</c:v>
+                  <c:v>7344531.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130</c:v>
+                  <c:v>11895250</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>19239781.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2790,7 +2805,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2828,7 +2843,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2907,7 +2922,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2945,7 +2960,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2987,7 +3002,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3024,7 +3039,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3033,7 +3048,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3095,7 +3110,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3183,7 +3198,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3234,34 +3249,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>625015625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>720000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>625735625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>626455625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>1252191250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3351,7 +3366,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3402,34 +3417,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>37031.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>294046.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>331078.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>625125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>956203.125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>1581328.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>2537531.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68</c:v>
+                  <c:v>4118859.375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>6656390.625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>10775250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3529,7 +3544,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3567,7 +3582,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3646,7 +3661,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3684,7 +3699,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3726,7 +3741,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3763,7 +3778,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3772,7 +3787,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3834,7 +3849,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3922,7 +3937,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3973,34 +3988,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>46.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>312.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>734.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>1781.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>4125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>12765.625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
+                  <c:v>26265.625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>53432.324000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4090,7 +4105,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4141,34 +4156,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>1890.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>10375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>44968.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>204546.875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>204556.875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>118</c:v>
+                  <c:v>204566.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>128</c:v>
+                  <c:v>204576.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>138</c:v>
+                  <c:v>204586.875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>148</c:v>
+                  <c:v>204596.875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>204606.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4268,7 +4283,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4306,7 +4321,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4385,7 +4400,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4423,7 +4438,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4465,7 +4480,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4502,7 +4517,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -7286,7 +7301,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7297,7 +7312,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7308,7 +7323,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7319,7 +7334,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7330,7 +7345,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7341,7 +7356,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7374,7 +7389,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7407,7 +7422,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7440,7 +7455,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7473,7 +7488,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9315915" cy="6086707"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7509,27 +7524,27 @@
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:D24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:D24" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A14:D24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7828,18 +7843,18 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7853,164 +7868,153 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
+        <v>484.375</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="4">
-        <v>4</v>
+        <v>15.625</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
       <c r="B3" s="4">
-        <v>20</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
+        <v>1843.75</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+        <v>46.875</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
       <c r="B4" s="4">
-        <v>30</v>
-      </c>
-      <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>3</v>
+        <v>8093.75</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
       <c r="B5" s="4">
-        <v>40</v>
-      </c>
-      <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+        <v>32015.625</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <v>312.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
       <c r="B6" s="4">
-        <v>50</v>
-      </c>
-      <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>138140.625</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <v>734.375</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
       <c r="B7" s="4">
-        <v>60</v>
+        <v>575031.25</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <v>625015625</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <v>1781.25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
       <c r="B8" s="4">
-        <v>70</v>
+        <v>720000</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <v>720000</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>69</v>
+        <v>4125</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
       <c r="B9" s="4">
-        <v>80</v>
+        <f>B8+B7</f>
+        <v>1295031.25</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
+        <f>C7+C8</f>
+        <v>625735625</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <v>12765.625</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
       <c r="B10" s="4">
-        <v>90</v>
+        <f>B8+B9</f>
+        <v>2015031.25</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
+        <f t="shared" ref="C9:C11" si="0">C9+C8</f>
+        <v>626455625</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>89</v>
+        <v>26265.625</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
       <c r="B11" s="4">
-        <v>100</v>
+        <f>B10+B8</f>
+        <v>2735031.25</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
+        <f t="shared" si="0"/>
+        <v>1252191250</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>99</v>
+        <v>53432.324000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -8024,161 +8028,165 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
       <c r="B15" s="4">
-        <v>50</v>
+        <v>39625</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>37031.25</v>
       </c>
       <c r="D15" s="4">
-        <v>35</v>
+        <v>1890.625</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
       <c r="B16" s="4">
-        <v>60</v>
+        <v>316906.25</v>
       </c>
       <c r="C16" s="4">
-        <v>4</v>
+        <v>294046.875</v>
       </c>
       <c r="D16" s="4">
-        <f>D15+43</f>
-        <v>78</v>
+        <v>10375</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
       <c r="B17" s="4">
-        <v>70</v>
+        <v>720000</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
+        <f t="shared" ref="C17:C24" si="1">C16+C15</f>
+        <v>331078.125</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
+        <v>44968.75</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
       <c r="B18" s="4">
-        <v>80</v>
+        <f>B17+B16</f>
+        <v>1036906.25</v>
       </c>
       <c r="C18" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>625125</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="3"/>
-        <v>98</v>
+        <v>204546.875</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
       <c r="B19" s="4">
-        <v>90</v>
+        <f>B17+B18</f>
+        <v>1756906.25</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>956203.125</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="3"/>
-        <v>108</v>
+        <f t="shared" ref="D17:D24" si="2">D18+10</f>
+        <v>204556.875</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
       <c r="B20" s="4">
-        <v>100</v>
+        <f t="shared" ref="B20:B24" si="3">B18+B19</f>
+        <v>2793812.5</v>
       </c>
       <c r="C20" s="4">
+        <f t="shared" si="1"/>
+        <v>1581328.125</v>
+      </c>
+      <c r="D20" s="4">
         <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
+        <v>204566.875</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
       <c r="B21" s="4">
-        <v>110</v>
+        <f t="shared" si="3"/>
+        <v>4550718.75</v>
       </c>
       <c r="C21" s="4">
+        <f t="shared" si="1"/>
+        <v>2537531.25</v>
+      </c>
+      <c r="D21" s="4">
         <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <v>204576.875</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
       <c r="B22" s="4">
-        <v>120</v>
+        <f t="shared" si="3"/>
+        <v>7344531.25</v>
       </c>
       <c r="C22" s="4">
+        <f t="shared" si="1"/>
+        <v>4118859.375</v>
+      </c>
+      <c r="D22" s="4">
         <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="3"/>
-        <v>138</v>
+        <v>204586.875</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
       <c r="B23" s="4">
-        <v>130</v>
+        <f t="shared" si="3"/>
+        <v>11895250</v>
       </c>
       <c r="C23" s="4">
+        <f t="shared" si="1"/>
+        <v>6656390.625</v>
+      </c>
+      <c r="D23" s="4">
         <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="3"/>
-        <v>148</v>
+        <v>204596.875</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>512000</v>
       </c>
       <c r="B24" s="4">
-        <v>140</v>
+        <f t="shared" si="3"/>
+        <v>19239781.25</v>
       </c>
       <c r="C24" s="4">
+        <f t="shared" si="1"/>
+        <v>10775250</v>
+      </c>
+      <c r="D24" s="4">
         <f t="shared" si="2"/>
-        <v>178</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>158</v>
+        <v>204606.875</v>
       </c>
     </row>
   </sheetData>
@@ -8191,12 +8199,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8411,15 +8416,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8444,10 +8453,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>